<commit_message>
Add lawn_* veg types to allometric.txt Update allometric workbook to reflect addition of ecalypt and lawn_*
</commit_message>
<xml_diff>
--- a/allometry/allometric_workbook.xlsx
+++ b/allometry/allometric_workbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15720" yWindow="0" windowWidth="12940" windowHeight="17580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3740" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>veg id</t>
   </si>
@@ -65,6 +65,18 @@
   </si>
   <si>
     <t>nonveg</t>
+  </si>
+  <si>
+    <t>eucalypt</t>
+  </si>
+  <si>
+    <t>lawn_10cm</t>
+  </si>
+  <si>
+    <t>lawn_5cm</t>
+  </si>
+  <si>
+    <t>lawn_2cm</t>
   </si>
 </sst>
 </file>
@@ -72,8 +84,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -132,15 +144,16 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -679,10 +692,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -869,7 +882,144 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4">
+        <v>11</v>
+      </c>
+      <c r="C6">
+        <v>8.74</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.32</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.3</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.73</v>
+      </c>
+      <c r="H6">
+        <v>28.7</v>
+      </c>
+      <c r="I6">
+        <v>139.69999999999999</v>
+      </c>
+      <c r="J6">
+        <v>200</v>
+      </c>
+      <c r="K6">
+        <v>333.33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>31</v>
+      </c>
+      <c r="C7">
+        <v>17</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H7">
+        <v>27.7</v>
+      </c>
+      <c r="I7">
+        <v>47.8</v>
+      </c>
+      <c r="J7">
+        <v>250</v>
+      </c>
+      <c r="K7">
+        <v>333.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>32</v>
+      </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H8">
+        <v>27.7</v>
+      </c>
+      <c r="I8">
+        <v>47.8</v>
+      </c>
+      <c r="J8">
+        <v>250</v>
+      </c>
+      <c r="K8">
+        <v>333.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9">
+        <v>33</v>
+      </c>
+      <c r="C9">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="H9">
+        <v>27.7</v>
+      </c>
+      <c r="I9">
+        <v>47.8</v>
+      </c>
+      <c r="J9">
+        <v>250</v>
+      </c>
+      <c r="K9">
+        <v>333.33</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>